<commit_message>
added agustus report and main menu footer hidden
</commit_message>
<xml_diff>
--- a/excel/IGD2022.xlsx
+++ b/excel/IGD2022.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <f>SUM(B2:C2)</f>
+        <f t="shared" ref="D2:D9" si="0">SUM(B2:C2)</f>
         <v>28</v>
       </c>
     </row>
@@ -492,7 +492,7 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <f>SUM(B3:C3)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -507,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <f>SUM(B4:C4)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
@@ -522,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <f>SUM(B5:C5)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -537,7 +537,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <f>SUM(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
@@ -552,7 +552,7 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <f>SUM(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
@@ -567,13 +567,23 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <f>SUM(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+      <c r="B9">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added september month report
</commit_message>
<xml_diff>
--- a/excel/IGD2022.xlsx
+++ b/excel/IGD2022.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D9" si="0">SUM(B2:C2)</f>
+        <f t="shared" ref="D2:D10" si="0">SUM(B2:C2)</f>
         <v>28</v>
       </c>
     </row>
@@ -589,6 +589,16 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10">
+        <v>89</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
desember 2022 done. 2022 done happy new year!
</commit_message>
<xml_diff>
--- a/excel/IGD2022.xlsx
+++ b/excel/IGD2022.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zicoprmd\Desktop\reportigdpetir\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminz\Desktop\reportigdpetir\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F79CA7-0DE3-40F5-B127-3D2E9B5A0D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1500" windowWidth="21600" windowHeight="13890"/>
+    <workbookView xWindow="2190" yWindow="1590" windowWidth="21600" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -444,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -478,7 +479,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D12" si="0">SUM(B2:C2)</f>
+        <f t="shared" ref="D2:D13" si="0">SUM(B2:C2)</f>
         <v>28</v>
       </c>
     </row>
@@ -635,6 +636,16 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
+      </c>
+      <c r="B13">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added laporan obat UGD
</commit_message>
<xml_diff>
--- a/excel/IGD2022.xlsx
+++ b/excel/IGD2022.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminz\Desktop\reportigdpetir\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F79CA7-0DE3-40F5-B127-3D2E9B5A0D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3453EF6-9338-4425-875E-CB2D1AB5DCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1590" windowWidth="21600" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="825" windowWidth="21600" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
+    <sheet name="2023" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Bulan</t>
   </si>
@@ -448,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -651,4 +652,141 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D528824F-2A2D-4421-BE3D-F6883A8E2959}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D13" si="0">SUM(B2:C2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>